<commit_message>
started analysis of cervCancer and vertColumn wt ksom model
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
+++ b/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56849E0-0144-4C3A-85C6-43297FCE849B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C162B3FC-39F5-45FE-83C5-ECD3C9093185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
@@ -103,8 +103,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -448,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,9 +535,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,37 +556,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -928,14 +923,15 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -978,42 +974,90 @@
       <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="C3" s="33">
+        <v>0.92028985507246397</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0.91304347826086996</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0.92753623188405798</v>
+      </c>
+      <c r="F3" s="38">
+        <v>0.90579710144927505</v>
+      </c>
+      <c r="G3" s="38">
+        <v>0.90579710144927505</v>
+      </c>
+      <c r="H3" s="38">
+        <v>0.89492753623188404</v>
+      </c>
+      <c r="I3" s="38">
+        <v>0.90217391304347805</v>
+      </c>
+      <c r="J3" s="39">
+        <v>0.90217391304347805</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="40">
+        <v>0.91304347826086996</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.92391304347826098</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.92391304347826098</v>
+      </c>
+      <c r="F4" s="40">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0.92028985507246397</v>
+      </c>
+      <c r="H4" s="40">
+        <v>0.90942028985507295</v>
+      </c>
+      <c r="I4" s="40">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="J4" s="41">
+        <v>0.90942028985507295</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="40">
+        <v>0.90942028985507295</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0.92753623188405798</v>
+      </c>
+      <c r="E5" s="40">
+        <v>0.89492753623188404</v>
+      </c>
+      <c r="F5" s="19">
+        <v>0.92391304347826098</v>
+      </c>
+      <c r="G5" s="40">
+        <v>0.90942028985507295</v>
+      </c>
+      <c r="H5" s="40">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.92391304347826098</v>
+      </c>
+      <c r="J5" s="41">
+        <v>0.90579710144927505</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -1022,42 +1066,90 @@
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="40">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.92028985507246397</v>
+      </c>
+      <c r="E6" s="40">
+        <v>0.91304347826086996</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.934782608695652</v>
+      </c>
+      <c r="G6" s="40">
+        <v>0.90579710144927505</v>
+      </c>
+      <c r="H6" s="40">
+        <v>0.90217391304347805</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.92028985507246397</v>
+      </c>
+      <c r="J6" s="41">
+        <v>0.89855072463768104</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="45"/>
+      <c r="C7" s="19">
+        <v>0.92391304347826098</v>
+      </c>
+      <c r="D7" s="40">
+        <v>0.90217391304347805</v>
+      </c>
+      <c r="E7" s="40">
+        <v>0.91304347826086996</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.92028985507246397</v>
+      </c>
+      <c r="G7" s="40">
+        <v>0.89855072463768104</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.92028985507246397</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0.90217391304347805</v>
+      </c>
+      <c r="J7" s="41">
+        <v>0.91304347826086996</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="C8" s="42">
+        <v>0.89855072463768104</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0.92028985507246397</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0.90579710144927505</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0.92391304347826098</v>
+      </c>
+      <c r="G8" s="42">
+        <v>0.90942028985507295</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0.92391304347826098</v>
+      </c>
+      <c r="J8" s="43">
+        <v>0.89855072463768104</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1067,29 +1159,29 @@
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="37"/>
-      <c r="L11" s="36" t="s">
+      <c r="K11" s="36"/>
+      <c r="L11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="36" t="s">
+      <c r="M11" s="36"/>
+      <c r="N11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="38"/>
+      <c r="O11" s="37"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
@@ -1145,57 +1237,135 @@
       <c r="B13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="4"/>
+      <c r="C13" s="26">
+        <v>512</v>
+      </c>
+      <c r="D13" s="27">
+        <v>64</v>
+      </c>
+      <c r="E13" s="44">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="F13" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="27">
+        <v>1</v>
+      </c>
+      <c r="H13" s="27">
+        <v>256</v>
+      </c>
+      <c r="I13" s="27">
+        <v>4</v>
+      </c>
+      <c r="J13" s="27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K13" s="44">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="L13" s="44">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="M13" s="44">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="N13" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="O13" s="4">
+        <v>256</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="30"/>
+      <c r="C14" s="28">
+        <v>1</v>
+      </c>
+      <c r="D14" s="29">
+        <v>8</v>
+      </c>
+      <c r="E14" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="29">
+        <v>1</v>
+      </c>
+      <c r="H14" s="29">
+        <v>512</v>
+      </c>
+      <c r="I14" s="29">
+        <v>64</v>
+      </c>
+      <c r="J14" s="29">
+        <v>2.4</v>
+      </c>
+      <c r="K14" s="29">
+        <v>64</v>
+      </c>
+      <c r="L14" s="45">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="M14" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="N14" s="29">
+        <v>256</v>
+      </c>
+      <c r="O14" s="30">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18"/>
       <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="30"/>
+      <c r="C15" s="28">
+        <v>2</v>
+      </c>
+      <c r="D15" s="29">
+        <v>64</v>
+      </c>
+      <c r="E15" s="45">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F15" s="29">
+        <v>32</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="H15" s="29">
+        <v>8</v>
+      </c>
+      <c r="I15" s="29">
+        <v>8</v>
+      </c>
+      <c r="J15" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="K15" s="45">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="L15" s="45">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="M15" s="45">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="N15" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="O15" s="30">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
@@ -1204,57 +1374,135 @@
       <c r="B16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="30"/>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="29">
+        <v>64</v>
+      </c>
+      <c r="E16" s="45">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="F16" s="29">
+        <v>2</v>
+      </c>
+      <c r="G16" s="29">
+        <v>2</v>
+      </c>
+      <c r="H16" s="29">
+        <v>512</v>
+      </c>
+      <c r="I16" s="29">
+        <v>64</v>
+      </c>
+      <c r="J16" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="K16" s="29">
+        <v>1</v>
+      </c>
+      <c r="L16" s="45">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="M16" s="45">
+        <v>3.125E-2</v>
+      </c>
+      <c r="N16" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="O16" s="30">
+        <v>64</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="30"/>
+      <c r="C17" s="28">
+        <v>1024</v>
+      </c>
+      <c r="D17" s="29">
+        <v>32</v>
+      </c>
+      <c r="E17" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="F17" s="29">
+        <v>16</v>
+      </c>
+      <c r="G17" s="29">
+        <v>0.6</v>
+      </c>
+      <c r="H17" s="29">
+        <v>16</v>
+      </c>
+      <c r="I17" s="29">
+        <v>4</v>
+      </c>
+      <c r="J17" s="29">
+        <v>0.4</v>
+      </c>
+      <c r="K17" s="29">
+        <v>8</v>
+      </c>
+      <c r="L17" s="45">
+        <v>3.125E-2</v>
+      </c>
+      <c r="M17" s="45">
+        <v>-1.953125E-3</v>
+      </c>
+      <c r="N17" s="29">
+        <v>16</v>
+      </c>
+      <c r="O17" s="30">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="33"/>
+      <c r="C18" s="46">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D18" s="31">
+        <v>64</v>
+      </c>
+      <c r="E18" s="47">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="F18" s="31">
+        <v>32</v>
+      </c>
+      <c r="G18" s="31">
+        <v>0.8</v>
+      </c>
+      <c r="H18" s="31">
+        <v>64</v>
+      </c>
+      <c r="I18" s="31">
+        <v>64</v>
+      </c>
+      <c r="J18" s="31">
+        <v>2.4</v>
+      </c>
+      <c r="K18" s="47">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="L18" s="47">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="M18" s="47">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="N18" s="31">
+        <v>4</v>
+      </c>
+      <c r="O18" s="32">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1272,7 +1520,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:J8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,42 +1570,90 @@
       <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="49"/>
+      <c r="C3" s="33">
+        <v>0.88949275362318903</v>
+      </c>
+      <c r="D3" s="38">
+        <v>0.87065217391304395</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0.88985507246376805</v>
+      </c>
+      <c r="F3" s="38">
+        <v>0.86014492753623195</v>
+      </c>
+      <c r="G3" s="38">
+        <v>0.88840579710144896</v>
+      </c>
+      <c r="H3" s="38">
+        <v>0.87789855072463796</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0.89384057971014497</v>
+      </c>
+      <c r="J3" s="39">
+        <v>0.87644927536231898</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="40">
+        <v>0.88260869565217404</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.89130434782608703</v>
+      </c>
+      <c r="E4" s="40">
+        <v>0.87608695652173896</v>
+      </c>
+      <c r="F4" s="40">
+        <v>0.87608695652173896</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0.88876811594202898</v>
+      </c>
+      <c r="H4" s="40">
+        <v>0.88152173913043497</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.89130434782608703</v>
+      </c>
+      <c r="J4" s="41">
+        <v>0.88840579710144896</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="40">
+        <v>0.86557971014492696</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0.88297101449275395</v>
+      </c>
+      <c r="E5" s="40">
+        <v>0.87391304347826104</v>
+      </c>
+      <c r="F5" s="40">
+        <v>0.79528985507246397</v>
+      </c>
+      <c r="G5" s="40">
+        <v>0.85942028985507302</v>
+      </c>
+      <c r="H5" s="19">
+        <v>0.88623188405797104</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.87898550724637703</v>
+      </c>
+      <c r="J5" s="41">
+        <v>0.85688405797101497</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -1366,42 +1662,90 @@
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="19">
+        <v>0.89384057971014497</v>
+      </c>
+      <c r="D6" s="40">
+        <v>0.88442028985507304</v>
+      </c>
+      <c r="E6" s="40">
+        <v>0.88478260869565195</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.90108695652173898</v>
+      </c>
+      <c r="G6" s="40">
+        <v>0.88115942028985506</v>
+      </c>
+      <c r="H6" s="40">
+        <v>0.88478260869565195</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.89746376811594197</v>
+      </c>
+      <c r="J6" s="41">
+        <v>0.88695652173912998</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="45"/>
+      <c r="C7" s="19">
+        <v>0.89384057971014497</v>
+      </c>
+      <c r="D7" s="40">
+        <v>0.88224637681159401</v>
+      </c>
+      <c r="E7" s="40">
+        <v>0.88659420289855095</v>
+      </c>
+      <c r="F7" s="40">
+        <v>0.88442028985507304</v>
+      </c>
+      <c r="G7" s="40">
+        <v>0.87753623188405805</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.89818840579710202</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0.889130434782609</v>
+      </c>
+      <c r="J7" s="41">
+        <v>0.88768115942029002</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="C8" s="42">
+        <v>0.85615942028985503</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0.88586956521739102</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0.876811594202899</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0.89166666666666705</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0.88695652173912998</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0.87898550724637703</v>
+      </c>
+      <c r="I8" s="42">
+        <v>0.85181159420289898</v>
+      </c>
+      <c r="J8" s="43">
+        <v>0.86666666666666703</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1413,7 +1757,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:J8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,42 +1806,42 @@
       <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="49"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18"/>
       <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
@@ -1506,42 +1850,42 @@
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="44"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="48"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1602,14 +1946,14 @@
       <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="34"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="35"/>
+      <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
@@ -1742,14 +2086,14 @@
       <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="34"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="35"/>
+      <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>

</xml_diff>

<commit_message>
added files for result analysis of 3 datasets
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
+++ b/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C162B3FC-39F5-45FE-83C5-ECD3C9093185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3B8F4D-8611-4A77-B89A-3D7349D23F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_hp_best" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -449,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -547,6 +547,24 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,36 +572,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -922,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A889A0D-6079-4851-A2AA-AD4BB1CBB64D}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,19 +971,19 @@
       <c r="E3" s="33">
         <v>0.92753623188405798</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="6">
         <v>0.90579710144927505</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="6">
         <v>0.90579710144927505</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="6">
         <v>0.89492753623188404</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="6">
         <v>0.90217391304347805</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="35">
         <v>0.90217391304347805</v>
       </c>
     </row>
@@ -1004,7 +992,7 @@
       <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="7">
         <v>0.91304347826086996</v>
       </c>
       <c r="D4" s="19">
@@ -1013,19 +1001,19 @@
       <c r="E4" s="19">
         <v>0.92391304347826098</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="7">
         <v>0.91666666666666696</v>
       </c>
       <c r="G4" s="19">
         <v>0.92028985507246397</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4" s="7">
         <v>0.90942028985507295</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="7">
         <v>0.91666666666666696</v>
       </c>
-      <c r="J4" s="41">
+      <c r="J4" s="8">
         <v>0.90942028985507295</v>
       </c>
     </row>
@@ -1034,28 +1022,28 @@
       <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="7">
         <v>0.90942028985507295</v>
       </c>
       <c r="D5" s="19">
         <v>0.92753623188405798</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="7">
         <v>0.89492753623188404</v>
       </c>
       <c r="F5" s="19">
         <v>0.92391304347826098</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="7">
         <v>0.90942028985507295</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="7">
         <v>0.91666666666666696</v>
       </c>
       <c r="I5" s="19">
         <v>0.92391304347826098</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="8">
         <v>0.90579710144927505</v>
       </c>
     </row>
@@ -1066,28 +1054,28 @@
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="7">
         <v>0.91666666666666696</v>
       </c>
       <c r="D6" s="19">
         <v>0.92028985507246397</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="7">
         <v>0.91304347826086996</v>
       </c>
       <c r="F6" s="19">
         <v>0.934782608695652</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="7">
         <v>0.90579710144927505</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6" s="7">
         <v>0.90217391304347805</v>
       </c>
       <c r="I6" s="19">
         <v>0.92028985507246397</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="8">
         <v>0.89855072463768104</v>
       </c>
     </row>
@@ -1099,25 +1087,25 @@
       <c r="C7" s="19">
         <v>0.92391304347826098</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="7">
         <v>0.90217391304347805</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="7">
         <v>0.91304347826086996</v>
       </c>
       <c r="F7" s="19">
         <v>0.92028985507246397</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="7">
         <v>0.89855072463768104</v>
       </c>
       <c r="H7" s="19">
         <v>0.92028985507246397</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="7">
         <v>0.90217391304347805</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="8">
         <v>0.91304347826086996</v>
       </c>
     </row>
@@ -1126,28 +1114,28 @@
       <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="9">
         <v>0.89855072463768104</v>
       </c>
       <c r="D8" s="21">
         <v>0.92028985507246397</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="9">
         <v>0.90579710144927505</v>
       </c>
       <c r="F8" s="21">
         <v>0.92391304347826098</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="9">
         <v>0.90942028985507295</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="9">
         <v>0.91666666666666696</v>
       </c>
       <c r="I8" s="21">
         <v>0.92391304347826098</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="36">
         <v>0.89855072463768104</v>
       </c>
     </row>
@@ -1159,29 +1147,29 @@
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="35" t="s">
+      <c r="K11" s="42"/>
+      <c r="L11" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="36"/>
-      <c r="N11" s="35" t="s">
+      <c r="M11" s="42"/>
+      <c r="N11" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="37"/>
+      <c r="O11" s="43"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
@@ -1243,7 +1231,7 @@
       <c r="D13" s="27">
         <v>64</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="37">
         <v>1.5625E-2</v>
       </c>
       <c r="F13" s="27">
@@ -1261,13 +1249,13 @@
       <c r="J13" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K13" s="44">
+      <c r="K13" s="37">
         <v>9.765625E-4</v>
       </c>
-      <c r="L13" s="44">
+      <c r="L13" s="37">
         <v>3.90625E-3</v>
       </c>
-      <c r="M13" s="44">
+      <c r="M13" s="37">
         <v>1.5625E-2</v>
       </c>
       <c r="N13" s="27">
@@ -1309,7 +1297,7 @@
       <c r="K14" s="29">
         <v>64</v>
       </c>
-      <c r="L14" s="45">
+      <c r="L14" s="38">
         <v>1.5625E-2</v>
       </c>
       <c r="M14" s="29">
@@ -1333,7 +1321,7 @@
       <c r="D15" s="29">
         <v>64</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="38">
         <v>6.25E-2</v>
       </c>
       <c r="F15" s="29">
@@ -1351,13 +1339,13 @@
       <c r="J15" s="29">
         <v>0.8</v>
       </c>
-      <c r="K15" s="45">
+      <c r="K15" s="38">
         <v>9.765625E-4</v>
       </c>
-      <c r="L15" s="45">
+      <c r="L15" s="38">
         <v>3.90625E-3</v>
       </c>
-      <c r="M15" s="45">
+      <c r="M15" s="38">
         <v>1.5625E-2</v>
       </c>
       <c r="N15" s="29">
@@ -1380,7 +1368,7 @@
       <c r="D16" s="29">
         <v>64</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="38">
         <v>7.8125E-3</v>
       </c>
       <c r="F16" s="29">
@@ -1401,10 +1389,10 @@
       <c r="K16" s="29">
         <v>1</v>
       </c>
-      <c r="L16" s="45">
+      <c r="L16" s="38">
         <v>3.90625E-3</v>
       </c>
-      <c r="M16" s="45">
+      <c r="M16" s="38">
         <v>3.125E-2</v>
       </c>
       <c r="N16" s="29">
@@ -1446,10 +1434,10 @@
       <c r="K17" s="29">
         <v>8</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="38">
         <v>3.125E-2</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M17" s="38">
         <v>-1.953125E-3</v>
       </c>
       <c r="N17" s="29">
@@ -1464,13 +1452,13 @@
       <c r="B18" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="39">
         <v>3.90625E-3</v>
       </c>
       <c r="D18" s="31">
         <v>64</v>
       </c>
-      <c r="E18" s="47">
+      <c r="E18" s="40">
         <v>3.90625E-3</v>
       </c>
       <c r="F18" s="31">
@@ -1488,13 +1476,13 @@
       <c r="J18" s="31">
         <v>2.4</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="40">
         <v>3.90625E-3</v>
       </c>
-      <c r="L18" s="47">
+      <c r="L18" s="40">
         <v>3.90625E-3</v>
       </c>
-      <c r="M18" s="47">
+      <c r="M18" s="40">
         <v>1.953125E-3</v>
       </c>
       <c r="N18" s="31">
@@ -1519,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C2E4AB-28B4-4560-9CA9-8AF5549FD7E4}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1573,25 +1561,25 @@
       <c r="C3" s="33">
         <v>0.88949275362318903</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="6">
         <v>0.87065217391304395</v>
       </c>
       <c r="E3" s="33">
         <v>0.88985507246376805</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="6">
         <v>0.86014492753623195</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="6">
         <v>0.88840579710144896</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="6">
         <v>0.87789855072463796</v>
       </c>
       <c r="I3" s="33">
         <v>0.89384057971014497</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="35">
         <v>0.87644927536231898</v>
       </c>
     </row>
@@ -1600,28 +1588,28 @@
       <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="7">
         <v>0.88260869565217404</v>
       </c>
       <c r="D4" s="19">
         <v>0.89130434782608703</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="7">
         <v>0.87608695652173896</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="7">
         <v>0.87608695652173896</v>
       </c>
       <c r="G4" s="19">
         <v>0.88876811594202898</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4" s="7">
         <v>0.88152173913043497</v>
       </c>
       <c r="I4" s="19">
         <v>0.89130434782608703</v>
       </c>
-      <c r="J4" s="41">
+      <c r="J4" s="8">
         <v>0.88840579710144896</v>
       </c>
     </row>
@@ -1630,19 +1618,19 @@
       <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="7">
         <v>0.86557971014492696</v>
       </c>
       <c r="D5" s="19">
         <v>0.88297101449275395</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="7">
         <v>0.87391304347826104</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="7">
         <v>0.79528985507246397</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="7">
         <v>0.85942028985507302</v>
       </c>
       <c r="H5" s="19">
@@ -1651,7 +1639,7 @@
       <c r="I5" s="19">
         <v>0.87898550724637703</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="8">
         <v>0.85688405797101497</v>
       </c>
     </row>
@@ -1665,25 +1653,25 @@
       <c r="C6" s="19">
         <v>0.89384057971014497</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="7">
         <v>0.88442028985507304</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="7">
         <v>0.88478260869565195</v>
       </c>
       <c r="F6" s="19">
         <v>0.90108695652173898</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="7">
         <v>0.88115942028985506</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6" s="7">
         <v>0.88478260869565195</v>
       </c>
       <c r="I6" s="19">
         <v>0.89746376811594197</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="8">
         <v>0.88695652173912998</v>
       </c>
     </row>
@@ -1695,16 +1683,16 @@
       <c r="C7" s="19">
         <v>0.89384057971014497</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="7">
         <v>0.88224637681159401</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="7">
         <v>0.88659420289855095</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="7">
         <v>0.88442028985507304</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="7">
         <v>0.87753623188405805</v>
       </c>
       <c r="H7" s="19">
@@ -1713,7 +1701,7 @@
       <c r="I7" s="19">
         <v>0.889130434782609</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="8">
         <v>0.88768115942029002</v>
       </c>
     </row>
@@ -1722,13 +1710,13 @@
       <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="9">
         <v>0.85615942028985503</v>
       </c>
       <c r="D8" s="21">
         <v>0.88586956521739102</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="9">
         <v>0.876811594202899</v>
       </c>
       <c r="F8" s="21">
@@ -1737,13 +1725,13 @@
       <c r="G8" s="21">
         <v>0.88695652173912998</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="9">
         <v>0.87898550724637703</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="9">
         <v>0.85181159420289898</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="36">
         <v>0.86666666666666703</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added acc std to ksom result analysis
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
+++ b/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab\results_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3B8F4D-8611-4A77-B89A-3D7349D23F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DC1FE0-3152-4C8B-BDD7-7E6BF7310B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_hp_best" sheetId="1" r:id="rId1"/>
     <sheet name="acc_mean" sheetId="2" r:id="rId2"/>
     <sheet name="acc_median" sheetId="5" r:id="rId3"/>
-    <sheet name="MCC" sheetId="3" r:id="rId4"/>
-    <sheet name="F1S" sheetId="4" r:id="rId5"/>
+    <sheet name="acc_std" sheetId="6" r:id="rId4"/>
+    <sheet name="MCC" sheetId="3" r:id="rId5"/>
+    <sheet name="F1S" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="19">
   <si>
     <t>Algorithm</t>
   </si>
@@ -449,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,6 +573,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1507,7 +1526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C2E4AB-28B4-4560-9CA9-8AF5549FD7E4}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1881,6 +1900,243 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A0A9BB-556C-4854-9DC7-E1CFB9D16510}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="44">
+        <v>1.64046832212634E-2</v>
+      </c>
+      <c r="D3" s="44">
+        <v>5.20039389966842E-2</v>
+      </c>
+      <c r="E3" s="44">
+        <v>1.64002369050898E-2</v>
+      </c>
+      <c r="F3" s="44">
+        <v>5.4232298036704103E-2</v>
+      </c>
+      <c r="G3" s="44">
+        <v>1.39595973688888E-2</v>
+      </c>
+      <c r="H3" s="44">
+        <v>8.7174311268688794E-3</v>
+      </c>
+      <c r="I3" s="44">
+        <v>7.4547339913096401E-3</v>
+      </c>
+      <c r="J3" s="45">
+        <v>1.7950126814965401E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="46">
+        <v>1.56725876304428E-2</v>
+      </c>
+      <c r="D4" s="46">
+        <v>2.1604521521737099E-2</v>
+      </c>
+      <c r="E4" s="46">
+        <v>5.2665868154466701E-2</v>
+      </c>
+      <c r="F4" s="46">
+        <v>5.5602794451142301E-2</v>
+      </c>
+      <c r="G4" s="46">
+        <v>1.8399551351317101E-2</v>
+      </c>
+      <c r="H4" s="46">
+        <v>1.6563955725597799E-2</v>
+      </c>
+      <c r="I4" s="46">
+        <v>1.37702346026466E-2</v>
+      </c>
+      <c r="J4" s="47">
+        <v>1.87723277562565E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="46">
+        <v>4.9130992923833799E-2</v>
+      </c>
+      <c r="D5" s="46">
+        <v>2.7223518866281101E-2</v>
+      </c>
+      <c r="E5" s="46">
+        <v>2.5264361091773699E-2</v>
+      </c>
+      <c r="F5" s="46">
+        <v>0.19773781010695399</v>
+      </c>
+      <c r="G5" s="46">
+        <v>8.4157168410316396E-2</v>
+      </c>
+      <c r="H5" s="46">
+        <v>2.5914171028147501E-2</v>
+      </c>
+      <c r="I5" s="46">
+        <v>4.6058691542233902E-2</v>
+      </c>
+      <c r="J5" s="47">
+        <v>6.2575073351105695E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="46">
+        <v>1.7917593708360598E-2</v>
+      </c>
+      <c r="D6" s="46">
+        <v>2.0024285705531601E-2</v>
+      </c>
+      <c r="E6" s="46">
+        <v>3.4193890568476097E-2</v>
+      </c>
+      <c r="F6" s="46">
+        <v>1.7917593708360598E-2</v>
+      </c>
+      <c r="G6" s="46">
+        <v>1.3317921499604099E-2</v>
+      </c>
+      <c r="H6" s="46">
+        <v>1.6977085401744502E-2</v>
+      </c>
+      <c r="I6" s="46">
+        <v>1.2787112012141499E-2</v>
+      </c>
+      <c r="J6" s="47">
+        <v>1.15589237816477E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="46">
+        <v>1.9477797182196499E-2</v>
+      </c>
+      <c r="D7" s="46">
+        <v>2.01549749616892E-2</v>
+      </c>
+      <c r="E7" s="46">
+        <v>1.7254054502890699E-2</v>
+      </c>
+      <c r="F7" s="46">
+        <v>2.1499619943810701E-2</v>
+      </c>
+      <c r="G7" s="46">
+        <v>1.3535193938282E-2</v>
+      </c>
+      <c r="H7" s="46">
+        <v>9.8783116167529307E-3</v>
+      </c>
+      <c r="I7" s="46">
+        <v>1.0829232739835701E-2</v>
+      </c>
+      <c r="J7" s="47">
+        <v>1.5466483665296699E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="48">
+        <v>6.5708696914803799E-2</v>
+      </c>
+      <c r="D8" s="48">
+        <v>3.5592178812298002E-2</v>
+      </c>
+      <c r="E8" s="48">
+        <v>2.1939495319547E-2</v>
+      </c>
+      <c r="F8" s="48">
+        <v>2.0527848513355498E-2</v>
+      </c>
+      <c r="G8" s="48">
+        <v>1.80594933744142E-2</v>
+      </c>
+      <c r="H8" s="48">
+        <v>3.0081920403585899E-2</v>
+      </c>
+      <c r="I8" s="48">
+        <v>6.68835738306887E-2</v>
+      </c>
+      <c r="J8" s="49">
+        <v>3.4911529731105798E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF95E80-F9D6-4C97-A976-8D8517BE58EB}">
   <dimension ref="A1:J8"/>
   <sheetViews>
@@ -2020,7 +2276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B47BB03-5D51-4927-8C90-D8C37E699AAE}">
   <dimension ref="A1:J8"/>
   <sheetViews>

</xml_diff>

<commit_message>
merged xls files of ksom datasets vertColumn and WallFollow
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
+++ b/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598A28C6-7FD3-464E-AE9D-0957DB0EF275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA799CC6-6BB9-4749-9D5B-DB904D66539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="hp_best" sheetId="8" r:id="rId1"/>
@@ -570,6 +570,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -577,9 +580,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -921,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F55AC05-9805-4136-9A48-917B2964BC4B}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -939,29 +939,29 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="40" t="s">
+      <c r="K2" s="42"/>
+      <c r="L2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="40" t="s">
+      <c r="M2" s="42"/>
+      <c r="N2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="42"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -1299,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A889A0D-6079-4851-A2AA-AD4BB1CBB64D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1314,18 +1314,18 @@
       <c r="A2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="31" t="s">
@@ -1545,15 +1545,15 @@
       <c r="A11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
@@ -1798,15 +1798,15 @@
       <c r="A2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -2029,15 +2029,15 @@
       <c r="A11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
@@ -2281,15 +2281,15 @@
       <c r="A2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -2416,15 +2416,15 @@
       <c r="A11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
@@ -2669,15 +2669,15 @@
       <c r="A2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -2900,15 +2900,15 @@
       <c r="A11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
@@ -3152,15 +3152,15 @@
       <c r="A2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -3287,15 +3287,15 @@
       <c r="A11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
@@ -3539,15 +3539,15 @@
       <c r="A2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -3674,15 +3674,15 @@
       <c r="A11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">

</xml_diff>

<commit_message>
updated result analysis of ksom xls files
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
+++ b/results_analysis/ksom_cervicalCancer_02_hold_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA799CC6-6BB9-4749-9D5B-DB904D66539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CEFCC7-553C-4084-BC8A-14EAF36D0953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="hp_best" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="28">
   <si>
     <t>Algorithm</t>
   </si>
@@ -106,6 +106,27 @@
   <si>
     <t>HPO = Best</t>
   </si>
+  <si>
+    <t>Comparison: HPO=Best - HPO=1</t>
+  </si>
+  <si>
+    <t>Comparison: KSOM-EF - KSOM-GD</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>HPO=1</t>
+  </si>
+  <si>
+    <t>HPO=Best</t>
+  </si>
+  <si>
+    <t>Comparison: Labeling Strategies, HPO = 1</t>
+  </si>
+  <si>
+    <t>Comparison: Labeling Strategies, HPO = best</t>
+  </si>
 </sst>
 </file>
 
@@ -140,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -453,11 +474,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,11 +768,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1299,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A889A0D-6079-4851-A2AA-AD4BB1CBB64D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1782,19 +2040,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C2E4AB-28B4-4560-9CA9-8AF5549FD7E4}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.88671875" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
         <v>19</v>
       </c>
@@ -1807,8 +2070,20 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
       <c r="J2" s="43"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L2" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="43"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1839,8 +2114,38 @@
       <c r="J3" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -1871,8 +2176,46 @@
       <c r="J4" s="34">
         <v>0.87644927536231898</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="61">
+        <f>C4-C7</f>
+        <v>-4.3478260869559415E-3</v>
+      </c>
+      <c r="O4" s="61">
+        <f t="shared" ref="O4:U6" si="0">D4-D7</f>
+        <v>-1.3768115942029091E-2</v>
+      </c>
+      <c r="P4" s="61">
+        <f t="shared" si="0"/>
+        <v>5.0724637681160978E-3</v>
+      </c>
+      <c r="Q4" s="61">
+        <f t="shared" si="0"/>
+        <v>-4.0942028985507029E-2</v>
+      </c>
+      <c r="R4" s="61">
+        <f t="shared" si="0"/>
+        <v>7.246376811593902E-3</v>
+      </c>
+      <c r="S4" s="61">
+        <f t="shared" si="0"/>
+        <v>-6.8840579710139904E-3</v>
+      </c>
+      <c r="T4" s="61">
+        <f t="shared" si="0"/>
+        <v>-3.6231884057970065E-3</v>
+      </c>
+      <c r="U4" s="62">
+        <f t="shared" si="0"/>
+        <v>-1.0507246376810997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="15" t="s">
         <v>17</v>
@@ -1901,8 +2244,44 @@
       <c r="J5" s="8">
         <v>0.88840579710144896</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L5" s="11"/>
+      <c r="M5" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="61">
+        <f t="shared" ref="N5:N6" si="1">C5-C8</f>
+        <v>-1.1231884057970931E-2</v>
+      </c>
+      <c r="O5" s="61">
+        <f t="shared" si="0"/>
+        <v>9.0579710144930159E-3</v>
+      </c>
+      <c r="P5" s="61">
+        <f t="shared" si="0"/>
+        <v>-1.0507246376811996E-2</v>
+      </c>
+      <c r="Q5" s="61">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333340809E-3</v>
+      </c>
+      <c r="R5" s="61">
+        <f t="shared" si="0"/>
+        <v>1.1231884057970931E-2</v>
+      </c>
+      <c r="S5" s="61">
+        <f t="shared" si="0"/>
+        <v>-1.6666666666667052E-2</v>
+      </c>
+      <c r="T5" s="61">
+        <f t="shared" si="0"/>
+        <v>2.1739130434780263E-3</v>
+      </c>
+      <c r="U5" s="62">
+        <f t="shared" si="0"/>
+        <v>7.2463768115893501E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="15" t="s">
         <v>18</v>
@@ -1931,8 +2310,44 @@
       <c r="J6" s="8">
         <v>0.85688405797101497</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L6" s="11"/>
+      <c r="M6" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="61">
+        <f t="shared" si="1"/>
+        <v>9.4202898550719283E-3</v>
+      </c>
+      <c r="O6" s="61">
+        <f t="shared" si="0"/>
+        <v>-2.8985507246370723E-3</v>
+      </c>
+      <c r="P6" s="61">
+        <f t="shared" si="0"/>
+        <v>-2.8985507246379605E-3</v>
+      </c>
+      <c r="Q6" s="61">
+        <f t="shared" si="0"/>
+        <v>-9.6376811594203082E-2</v>
+      </c>
+      <c r="R6" s="61">
+        <f t="shared" si="0"/>
+        <v>-2.7536231884056961E-2</v>
+      </c>
+      <c r="S6" s="61">
+        <f t="shared" si="0"/>
+        <v>7.246376811594013E-3</v>
+      </c>
+      <c r="T6" s="61">
+        <f t="shared" si="0"/>
+        <v>2.7173913043478048E-2</v>
+      </c>
+      <c r="U6" s="62">
+        <f t="shared" si="0"/>
+        <v>-9.7826086956520619E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>2</v>
       </c>
@@ -1963,8 +2378,46 @@
       <c r="J7" s="8">
         <v>0.88695652173912998</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="63">
+        <f>C13-C16</f>
+        <v>2.4637681159429548E-3</v>
+      </c>
+      <c r="O7" s="63">
+        <f t="shared" ref="O7:U9" si="2">D13-D16</f>
+        <v>2.6449275362319113E-3</v>
+      </c>
+      <c r="P7" s="63">
+        <f t="shared" si="2"/>
+        <v>8.3333333333301951E-4</v>
+      </c>
+      <c r="Q7" s="63">
+        <f t="shared" si="2"/>
+        <v>5.7608695652179298E-3</v>
+      </c>
+      <c r="R7" s="63">
+        <f t="shared" si="2"/>
+        <v>1.8478260869559948E-3</v>
+      </c>
+      <c r="S7" s="63">
+        <f t="shared" si="2"/>
+        <v>-6.5217391304306371E-4</v>
+      </c>
+      <c r="T7" s="63">
+        <f t="shared" si="2"/>
+        <v>-1.1231884057970598E-3</v>
+      </c>
+      <c r="U7" s="64">
+        <f t="shared" si="2"/>
+        <v>5.579710144927974E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="15" t="s">
         <v>17</v>
@@ -1993,8 +2446,44 @@
       <c r="J8" s="8">
         <v>0.88768115942029002</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L8" s="11"/>
+      <c r="M8" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="63">
+        <f t="shared" ref="N8:N9" si="3">C14-C17</f>
+        <v>-5.5072463768109925E-3</v>
+      </c>
+      <c r="O8" s="63">
+        <f t="shared" si="2"/>
+        <v>1.0326086956521929E-2</v>
+      </c>
+      <c r="P8" s="63">
+        <f t="shared" si="2"/>
+        <v>4.6014492753629899E-3</v>
+      </c>
+      <c r="Q8" s="63">
+        <f t="shared" si="2"/>
+        <v>9.0579710144930159E-3</v>
+      </c>
+      <c r="R8" s="63">
+        <f t="shared" si="2"/>
+        <v>-5.5072463768109925E-3</v>
+      </c>
+      <c r="S8" s="63">
+        <f t="shared" si="2"/>
+        <v>-4.6594202898550985E-2</v>
+      </c>
+      <c r="T8" s="63">
+        <f t="shared" si="2"/>
+        <v>3.1159420289850193E-3</v>
+      </c>
+      <c r="U8" s="64">
+        <f t="shared" si="2"/>
+        <v>5.5797101449269748E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="16" t="s">
         <v>18</v>
@@ -2023,9 +2512,45 @@
       <c r="J9" s="35">
         <v>0.86666666666666703</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="12"/>
+      <c r="M9" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="65">
+        <f t="shared" si="3"/>
+        <v>3.2608695652192043E-4</v>
+      </c>
+      <c r="O9" s="65">
+        <f t="shared" si="2"/>
+        <v>1.6086956521738971E-2</v>
+      </c>
+      <c r="P9" s="65">
+        <f t="shared" si="2"/>
+        <v>-1.231884057971E-2</v>
+      </c>
+      <c r="Q9" s="65">
+        <f t="shared" si="2"/>
+        <v>-1.6195652173912944E-2</v>
+      </c>
+      <c r="R9" s="65">
+        <f t="shared" si="2"/>
+        <v>-1.1050724637680975E-2</v>
+      </c>
+      <c r="S9" s="65">
+        <f t="shared" si="2"/>
+        <v>9.1666666666659902E-3</v>
+      </c>
+      <c r="T9" s="65">
+        <f t="shared" si="2"/>
+        <v>-5.7971014492708139E-4</v>
+      </c>
+      <c r="U9" s="66">
+        <f t="shared" si="2"/>
+        <v>-6.8115942028980081E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="44" t="s">
         <v>20</v>
       </c>
@@ -2038,8 +2563,20 @@
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="43"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="43"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>0</v>
       </c>
@@ -2070,8 +2607,38 @@
       <c r="J12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>1</v>
       </c>
@@ -2081,10 +2648,10 @@
       <c r="C13" s="6">
         <v>0.88797101449275395</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="32">
         <v>0.89115942028985495</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="32">
         <v>0.88963768115941999</v>
       </c>
       <c r="F13" s="6">
@@ -2099,11 +2666,49 @@
       <c r="I13" s="6">
         <v>0.88797101449275395</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="33">
         <v>0.88916666666666699</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="52">
+        <f t="shared" ref="N13:U13" si="4">C4-MAX(C4:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="53">
+        <f t="shared" si="4"/>
+        <v>-2.0652173913043081E-2</v>
+      </c>
+      <c r="P13" s="53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="53">
+        <f t="shared" si="4"/>
+        <v>-1.5942028985507006E-2</v>
+      </c>
+      <c r="R13" s="53">
+        <f t="shared" si="4"/>
+        <v>-3.6231884058002262E-4</v>
+      </c>
+      <c r="S13" s="53">
+        <f t="shared" si="4"/>
+        <v>-8.3333333333330817E-3</v>
+      </c>
+      <c r="T13" s="53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="54">
+        <f t="shared" si="4"/>
+        <v>-1.1956521739129977E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="15" t="s">
         <v>17</v>
@@ -2117,7 +2722,7 @@
       <c r="E14" s="7">
         <v>0.88536231884058003</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="19">
         <v>0.88876811594202898</v>
       </c>
       <c r="G14" s="7">
@@ -2126,14 +2731,50 @@
       <c r="H14" s="7">
         <v>0.83902173913043498</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="19">
         <v>0.88764492753623203</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="68">
         <v>0.88702898550724596</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L14" s="11"/>
+      <c r="M14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="55">
+        <f t="shared" ref="N14:U14" si="5">C5-MAX(C4:C6)</f>
+        <v>-6.8840579710149896E-3</v>
+      </c>
+      <c r="O14" s="51">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="51">
+        <f t="shared" si="5"/>
+        <v>-1.3768115942029091E-2</v>
+      </c>
+      <c r="Q14" s="51">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="51">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="51">
+        <f t="shared" si="5"/>
+        <v>-4.7101449275360752E-3</v>
+      </c>
+      <c r="T14" s="51">
+        <f t="shared" si="5"/>
+        <v>-2.5362318840579379E-3</v>
+      </c>
+      <c r="U14" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="15" t="s">
         <v>18</v>
@@ -2141,7 +2782,7 @@
       <c r="C15" s="7">
         <v>0.87373188405797098</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="19">
         <v>0.89</v>
       </c>
       <c r="E15" s="7">
@@ -2153,17 +2794,53 @@
       <c r="G15" s="7">
         <v>0.86536231884058001</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="19">
         <v>0.879565217391304</v>
       </c>
       <c r="I15" s="7">
         <v>0.87289855072463796</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="68">
         <v>0.87394927536231903</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L15" s="11"/>
+      <c r="M15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="55">
+        <f>C6-MAX(C4:C6)</f>
+        <v>-2.3913043478262064E-2</v>
+      </c>
+      <c r="O15" s="51">
+        <f t="shared" ref="O15:U15" si="6">D6-MAX(D4:D6)</f>
+        <v>-8.3333333333330817E-3</v>
+      </c>
+      <c r="P15" s="51">
+        <f t="shared" si="6"/>
+        <v>-1.5942028985507006E-2</v>
+      </c>
+      <c r="Q15" s="51">
+        <f t="shared" si="6"/>
+        <v>-8.0797101449274988E-2</v>
+      </c>
+      <c r="R15" s="51">
+        <f t="shared" si="6"/>
+        <v>-2.9347826086955964E-2</v>
+      </c>
+      <c r="S15" s="51">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="51">
+        <f t="shared" si="6"/>
+        <v>-1.4855072463767938E-2</v>
+      </c>
+      <c r="U15" s="57">
+        <f t="shared" si="6"/>
+        <v>-3.152173913043399E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
@@ -2173,10 +2850,10 @@
       <c r="C16" s="7">
         <v>0.885507246376811</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="19">
         <v>0.88851449275362304</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="19">
         <v>0.88880434782608697</v>
       </c>
       <c r="F16" s="7">
@@ -2188,14 +2865,52 @@
       <c r="H16" s="7">
         <v>0.88724637681159402</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="19">
         <v>0.88909420289855101</v>
       </c>
       <c r="J16" s="8">
         <v>0.88358695652173902</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" s="55">
+        <f>C7-MAX(C7:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="51">
+        <f t="shared" ref="O16:U16" si="7">D7-MAX(D7:D9)</f>
+        <v>-1.449275362317981E-3</v>
+      </c>
+      <c r="P16" s="51">
+        <f t="shared" si="7"/>
+        <v>-1.8115942028990029E-3</v>
+      </c>
+      <c r="Q16" s="51">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="51">
+        <f t="shared" si="7"/>
+        <v>-5.7971014492749218E-3</v>
+      </c>
+      <c r="S16" s="51">
+        <f t="shared" si="7"/>
+        <v>-1.3405797101450068E-2</v>
+      </c>
+      <c r="T16" s="51">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="57">
+        <f t="shared" si="7"/>
+        <v>-7.2463768116004523E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="15" t="s">
         <v>17</v>
@@ -2212,20 +2927,56 @@
       <c r="F17" s="7">
         <v>0.87971014492753596</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="19">
         <v>0.88728260869565201</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="19">
         <v>0.88561594202898597</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="19">
         <v>0.88452898550724701</v>
       </c>
       <c r="J17" s="8">
         <v>0.88144927536231898</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L17" s="11"/>
+      <c r="M17" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="55">
+        <f>C8-MAX(C7:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="51">
+        <f t="shared" ref="O17:U17" si="8">D8-MAX(D7:D9)</f>
+        <v>-3.6231884057970065E-3</v>
+      </c>
+      <c r="P17" s="51">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="51">
+        <f t="shared" si="8"/>
+        <v>-1.6666666666665941E-2</v>
+      </c>
+      <c r="R17" s="51">
+        <f t="shared" si="8"/>
+        <v>-9.4202898550719283E-3</v>
+      </c>
+      <c r="S17" s="51">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T17" s="51">
+        <f t="shared" si="8"/>
+        <v>-8.3333333333329707E-3</v>
+      </c>
+      <c r="U17" s="57">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="16" t="s">
         <v>18</v>
@@ -2236,10 +2987,10 @@
       <c r="D18" s="9">
         <v>0.87391304347826104</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="21">
         <v>0.881376811594203</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="21">
         <v>0.88188405797101399</v>
       </c>
       <c r="G18" s="9">
@@ -2251,16 +3002,614 @@
       <c r="I18" s="9">
         <v>0.87347826086956504</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="20">
         <v>0.88076086956521704</v>
       </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="58">
+        <f>C9-MAX(C7:C9)</f>
+        <v>-3.7681159420289934E-2</v>
+      </c>
+      <c r="O18" s="59">
+        <f t="shared" ref="O18:U18" si="9">D9-MAX(D7:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="59">
+        <f t="shared" si="9"/>
+        <v>-9.7826086956519509E-3</v>
+      </c>
+      <c r="Q18" s="59">
+        <f t="shared" si="9"/>
+        <v>-9.4202898550719283E-3</v>
+      </c>
+      <c r="R18" s="59">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="59">
+        <f t="shared" si="9"/>
+        <v>-1.9202898550724989E-2</v>
+      </c>
+      <c r="T18" s="59">
+        <f t="shared" si="9"/>
+        <v>-4.5652173913042993E-2</v>
+      </c>
+      <c r="U18" s="60">
+        <f t="shared" si="9"/>
+        <v>-2.1014492753622993E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="43"/>
+      <c r="L20" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="43"/>
+    </row>
+    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="52">
+        <f>C13-C4</f>
+        <v>-1.5217391304350736E-3</v>
+      </c>
+      <c r="D22" s="53">
+        <f t="shared" ref="D22:J22" si="10">D13-D4</f>
+        <v>2.0507246376811006E-2</v>
+      </c>
+      <c r="E22" s="53">
+        <f t="shared" si="10"/>
+        <v>-2.1739130434805798E-4</v>
+      </c>
+      <c r="F22" s="53">
+        <f t="shared" si="10"/>
+        <v>2.7753623188406018E-2</v>
+      </c>
+      <c r="G22" s="53">
+        <f t="shared" si="10"/>
+        <v>3.6231884058002262E-4</v>
+      </c>
+      <c r="H22" s="53">
+        <f t="shared" si="10"/>
+        <v>8.6956521739129933E-3</v>
+      </c>
+      <c r="I22" s="53">
+        <f t="shared" si="10"/>
+        <v>-5.8695652173910151E-3</v>
+      </c>
+      <c r="J22" s="54">
+        <f t="shared" si="10"/>
+        <v>1.2717391304348014E-2</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="52">
+        <f>C13-MAX(C13:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="53">
+        <f t="shared" ref="O22:U22" si="11">D13-MAX(D13:D15)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="53">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="53">
+        <f t="shared" si="11"/>
+        <v>-8.6956521739101067E-4</v>
+      </c>
+      <c r="R22" s="53">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="53">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="53">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="54">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="55">
+        <f t="shared" ref="C23:J23" si="12">C14-C5</f>
+        <v>-4.4927536231880172E-3</v>
+      </c>
+      <c r="D23" s="56">
+        <f t="shared" si="12"/>
+        <v>-5.2173913043480624E-3</v>
+      </c>
+      <c r="E23" s="56">
+        <f t="shared" si="12"/>
+        <v>9.2753623188410739E-3</v>
+      </c>
+      <c r="F23" s="56">
+        <f t="shared" si="12"/>
+        <v>1.2681159420290022E-2</v>
+      </c>
+      <c r="G23" s="56">
+        <f t="shared" si="12"/>
+        <v>-6.9927536231879639E-3</v>
+      </c>
+      <c r="H23" s="56">
+        <f t="shared" si="12"/>
+        <v>-4.2499999999999982E-2</v>
+      </c>
+      <c r="I23" s="56">
+        <f t="shared" si="12"/>
+        <v>-3.6594202898549977E-3</v>
+      </c>
+      <c r="J23" s="57">
+        <f t="shared" si="12"/>
+        <v>-1.3768115942029979E-3</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="55">
+        <f>C14-MAX(C13:C15)</f>
+        <v>-9.8550724637679332E-3</v>
+      </c>
+      <c r="O23" s="51">
+        <f t="shared" ref="O23:U23" si="13">D14-MAX(D13:D15)</f>
+        <v>-5.0724637681159868E-3</v>
+      </c>
+      <c r="P23" s="51">
+        <f t="shared" si="13"/>
+        <v>-4.2753623188399592E-3</v>
+      </c>
+      <c r="Q23" s="51">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="51">
+        <f t="shared" si="13"/>
+        <v>-6.9927536231879639E-3</v>
+      </c>
+      <c r="S23" s="51">
+        <f t="shared" si="13"/>
+        <v>-4.7572463768115969E-2</v>
+      </c>
+      <c r="T23" s="51">
+        <f t="shared" si="13"/>
+        <v>-3.2608695652192043E-4</v>
+      </c>
+      <c r="U23" s="57">
+        <f t="shared" si="13"/>
+        <v>-2.1376811594210343E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="11"/>
+      <c r="B24" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="55">
+        <f t="shared" ref="C24:J24" si="14">C15-C6</f>
+        <v>8.1521739130440141E-3</v>
+      </c>
+      <c r="D24" s="56">
+        <f t="shared" si="14"/>
+        <v>7.0289855072460661E-3</v>
+      </c>
+      <c r="E24" s="56">
+        <f t="shared" si="14"/>
+        <v>-4.8550724637680398E-3</v>
+      </c>
+      <c r="F24" s="56">
+        <f t="shared" si="14"/>
+        <v>7.0398550724637077E-2</v>
+      </c>
+      <c r="G24" s="56">
+        <f t="shared" si="14"/>
+        <v>5.9420289855069974E-3</v>
+      </c>
+      <c r="H24" s="56">
+        <f t="shared" si="14"/>
+        <v>-6.6666666666670427E-3</v>
+      </c>
+      <c r="I24" s="56">
+        <f t="shared" si="14"/>
+        <v>-6.0869565217390731E-3</v>
+      </c>
+      <c r="J24" s="57">
+        <f t="shared" si="14"/>
+        <v>1.7065217391304066E-2</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="55">
+        <f>C15-MAX(C13:C15)</f>
+        <v>-1.4239130434782976E-2</v>
+      </c>
+      <c r="O24" s="51">
+        <f t="shared" ref="O24:U24" si="15">D15-MAX(D13:D15)</f>
+        <v>-1.1594202898549399E-3</v>
+      </c>
+      <c r="P24" s="51">
+        <f t="shared" si="15"/>
+        <v>-2.0579710144926988E-2</v>
+      </c>
+      <c r="Q24" s="51">
+        <f t="shared" si="15"/>
+        <v>-2.3079710144927934E-2</v>
+      </c>
+      <c r="R24" s="51">
+        <f t="shared" si="15"/>
+        <v>-2.3405797101448966E-2</v>
+      </c>
+      <c r="S24" s="51">
+        <f t="shared" si="15"/>
+        <v>-7.0289855072469543E-3</v>
+      </c>
+      <c r="T24" s="51">
+        <f t="shared" si="15"/>
+        <v>-1.5072463768115996E-2</v>
+      </c>
+      <c r="U24" s="57">
+        <f t="shared" si="15"/>
+        <v>-1.521739130434796E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="55">
+        <f t="shared" ref="C25:J25" si="16">C16-C7</f>
+        <v>-8.3333333333339699E-3</v>
+      </c>
+      <c r="D25" s="56">
+        <f t="shared" si="16"/>
+        <v>4.0942028985500034E-3</v>
+      </c>
+      <c r="E25" s="56">
+        <f t="shared" si="16"/>
+        <v>4.0217391304350203E-3</v>
+      </c>
+      <c r="F25" s="56">
+        <f t="shared" si="16"/>
+        <v>-1.894927536231894E-2</v>
+      </c>
+      <c r="G25" s="56">
+        <f t="shared" si="16"/>
+        <v>5.7608695652179298E-3</v>
+      </c>
+      <c r="H25" s="56">
+        <f t="shared" si="16"/>
+        <v>2.4637681159420666E-3</v>
+      </c>
+      <c r="I25" s="56">
+        <f t="shared" si="16"/>
+        <v>-8.3695652173909618E-3</v>
+      </c>
+      <c r="J25" s="57">
+        <f t="shared" si="16"/>
+        <v>-3.3695652173909574E-3</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="55">
+        <f>C16-MAX(C16:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="51">
+        <f t="shared" ref="O25:U25" si="17">D16-MAX(D16:D18)</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="51">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="51">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="51">
+        <f t="shared" si="17"/>
+        <v>-3.6231884057902342E-4</v>
+      </c>
+      <c r="S25" s="51">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="51">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="57">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="55">
+        <f t="shared" ref="C26:J26" si="18">C17-C8</f>
+        <v>-1.0217391304347956E-2</v>
+      </c>
+      <c r="D26" s="56">
+        <f t="shared" si="18"/>
+        <v>-6.4855072463769758E-3</v>
+      </c>
+      <c r="E26" s="56">
+        <f t="shared" si="18"/>
+        <v>-5.8333333333339121E-3</v>
+      </c>
+      <c r="F26" s="56">
+        <f t="shared" si="18"/>
+        <v>-4.7101449275370744E-3</v>
+      </c>
+      <c r="G26" s="56">
+        <f t="shared" si="18"/>
+        <v>9.7463768115939597E-3</v>
+      </c>
+      <c r="H26" s="56">
+        <f t="shared" si="18"/>
+        <v>-1.2572463768116049E-2</v>
+      </c>
+      <c r="I26" s="56">
+        <f t="shared" si="18"/>
+        <v>-4.6014492753619907E-3</v>
+      </c>
+      <c r="J26" s="57">
+        <f t="shared" si="18"/>
+        <v>-6.2318840579710377E-3</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="55">
+        <f>C17-MAX(C16:C18)</f>
+        <v>-1.884057971013986E-3</v>
+      </c>
+      <c r="O26" s="51">
+        <f t="shared" ref="O26:U26" si="19">D17-MAX(D16:D18)</f>
+        <v>-1.2753623188406005E-2</v>
+      </c>
+      <c r="P26" s="51">
+        <f t="shared" si="19"/>
+        <v>-8.0434782608699296E-3</v>
+      </c>
+      <c r="Q26" s="51">
+        <f t="shared" si="19"/>
+        <v>-2.4275362318840754E-3</v>
+      </c>
+      <c r="R26" s="51">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="S26" s="51">
+        <f t="shared" si="19"/>
+        <v>-1.6304347826080479E-3</v>
+      </c>
+      <c r="T26" s="51">
+        <f t="shared" si="19"/>
+        <v>-4.5652173913039995E-3</v>
+      </c>
+      <c r="U26" s="57">
+        <f t="shared" si="19"/>
+        <v>-2.1376811594200351E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="12"/>
+      <c r="B27" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="58">
+        <f t="shared" ref="C27:J27" si="20">C18-C9</f>
+        <v>1.7246376811594022E-2</v>
+      </c>
+      <c r="D27" s="59">
+        <f t="shared" si="20"/>
+        <v>-1.1956521739129977E-2</v>
+      </c>
+      <c r="E27" s="59">
+        <f t="shared" si="20"/>
+        <v>4.5652173913039995E-3</v>
+      </c>
+      <c r="F27" s="59">
+        <f t="shared" si="20"/>
+        <v>-9.7826086956530611E-3</v>
+      </c>
+      <c r="G27" s="59">
+        <f t="shared" si="20"/>
+        <v>-1.0543478260868988E-2</v>
+      </c>
+      <c r="H27" s="59">
+        <f t="shared" si="20"/>
+        <v>-8.5869565217390198E-3</v>
+      </c>
+      <c r="I27" s="59">
+        <f t="shared" si="20"/>
+        <v>2.1666666666666057E-2</v>
+      </c>
+      <c r="J27" s="60">
+        <f t="shared" si="20"/>
+        <v>1.4094202898550012E-2</v>
+      </c>
+      <c r="L27" s="12"/>
+      <c r="M27" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N27" s="58">
+        <f>C18-MAX(C16:C18)</f>
+        <v>-1.2101449275361942E-2</v>
+      </c>
+      <c r="O27" s="59">
+        <f t="shared" ref="O27:U27" si="21">D18-MAX(D16:D18)</f>
+        <v>-1.4601449275362E-2</v>
+      </c>
+      <c r="P27" s="59">
+        <f t="shared" si="21"/>
+        <v>-7.4275362318839688E-3</v>
+      </c>
+      <c r="Q27" s="59">
+        <f t="shared" si="21"/>
+        <v>-2.5362318840604914E-4</v>
+      </c>
+      <c r="R27" s="59">
+        <f t="shared" si="21"/>
+        <v>-1.086956521739102E-2</v>
+      </c>
+      <c r="S27" s="59">
+        <f t="shared" si="21"/>
+        <v>-1.6847826086956008E-2</v>
+      </c>
+      <c r="T27" s="59">
+        <f t="shared" si="21"/>
+        <v>-1.5615942028985974E-2</v>
+      </c>
+      <c r="U27" s="60">
+        <f t="shared" si="21"/>
+        <v>-2.8260869565219782E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D29" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="L11:U11"/>
+    <mergeCell ref="L20:U20"/>
   </mergeCells>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>"$C$13&gt;=MAIOR($C$13:$J$13,3)"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>"$C$13&gt;=MAIOR($C$13:$J$13,3)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>"$D$13&gt;=MAIOR($C$13:$J$13,3)"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2268,7 +3617,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C1C768-E5FF-4F1E-85F6-B83F97AC222C}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>